<commit_message>
mise à jour nb de mux necessaire"
</commit_message>
<xml_diff>
--- a/Presentation/feuille de course.xlsx
+++ b/Presentation/feuille de course.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,7 +11,7 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -80,7 +80,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="_-* #,##0.000\ [$€-40C]_-;\-* #,##0.000\ [$€-40C]_-;_-* &quot;-&quot;??\ [$€-40C]_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.000\ [$€-40C]_-;\-* #,##0.000\ [$€-40C]_-;_-* &quot;-&quot;??\ [$€-40C]_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -271,11 +271,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -337,7 +337,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -372,7 +372,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -584,7 +584,7 @@
   <dimension ref="B2:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,7 +685,7 @@
         <v>16</v>
       </c>
       <c r="C6" s="8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>18</v>
@@ -698,7 +698,7 @@
       </c>
       <c r="G6" s="14">
         <f t="shared" si="0"/>
-        <v>2.6120000000000001</v>
+        <v>3.9180000000000001</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
@@ -810,7 +810,7 @@
       <c r="F17" s="4"/>
       <c r="G17" s="18">
         <f>SUM(G3:G15)</f>
-        <v>17.236000000000001</v>
+        <v>18.542000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mise a jour feuille de course
</commit_message>
<xml_diff>
--- a/Presentation/feuille de course.xlsx
+++ b/Presentation/feuille de course.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Composant</t>
   </si>
@@ -82,6 +82,30 @@
   </si>
   <si>
     <t>http://fr.farnell.com/texas-instruments/sn74lvc3g17dctr/circuit-logique-trigger-de-schmitt/dp/1236391</t>
+  </si>
+  <si>
+    <t>http://fr.rs-online.com/web/p/drivers-de-moteur/7570499/?searchTerm=LB1836M-TLM-E&amp;relevancy-data=636F3D3226696E3D4931384E4B6E6F776E41734D504E266C753D6672266D6D3D6D61746368616C6C7061727469616C26706D3D5E5B5C707B4C7D5C707B4E647D2D2C2F255C2E5D2B2426706F3D313326736E3D592673743D4D414E5F504152545F4E554D4245522677633D424F5448267573743D4C42313833364D2D544C4D2D4526&amp;sra=p</t>
+  </si>
+  <si>
+    <t>pont en H (v2,0)</t>
+  </si>
+  <si>
+    <t>LB1836M-TLM-E</t>
+  </si>
+  <si>
+    <t> SN74AHC14N</t>
+  </si>
+  <si>
+    <t>http://www.ti.com/lit/ds/symlink/sn74ahc14.pdf</t>
+  </si>
+  <si>
+    <t>MCP3008</t>
+  </si>
+  <si>
+    <t>CAN SPI</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/datasheets/MCP3008.pdf</t>
   </si>
 </sst>
 </file>
@@ -91,7 +115,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.000\ [$€-40C]_-;\-* #,##0.000\ [$€-40C]_-;_-* &quot;-&quot;??\ [$€-40C]_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +145,19 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -261,7 +298,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -285,6 +322,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -593,14 +632,14 @@
   <dimension ref="B2:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="29.5703125" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="51" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
     <col min="7" max="7" width="12.42578125" customWidth="1"/>
@@ -626,12 +665,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>5</v>
@@ -644,7 +683,7 @@
       </c>
       <c r="G3" s="14">
         <f>F3*C3</f>
-        <v>4.38</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
@@ -668,12 +707,12 @@
         <v>0.76400000000000001</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>13</v>
@@ -686,7 +725,7 @@
       </c>
       <c r="G5" s="14">
         <f t="shared" si="0"/>
-        <v>9.48</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
@@ -710,12 +749,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="8">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>20</v>
@@ -728,18 +767,28 @@
       </c>
       <c r="G7" s="14">
         <f t="shared" si="0"/>
-        <v>1.19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="14"/>
+      <c r="B8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="8">
+        <v>2</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="14">
+        <v>2.65</v>
+      </c>
       <c r="G8" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -753,22 +802,38 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="8"/>
+    <row r="10" spans="2:7" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="B10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="8">
+        <v>1</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="F10" s="14"/>
       <c r="G10" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="8"/>
+    <row r="11" spans="2:7" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="B11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="8">
+        <v>1</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="F11" s="14"/>
       <c r="G11" s="14">
         <f t="shared" si="0"/>
@@ -829,7 +894,7 @@
       <c r="F17" s="4"/>
       <c r="G17" s="18">
         <f>SUM(G3:G15)</f>
-        <v>15.814</v>
+        <v>6.0640000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -839,6 +904,7 @@
     <hyperlink ref="E3" r:id="rId2"/>
     <hyperlink ref="E6" r:id="rId3"/>
     <hyperlink ref="E7" r:id="rId4"/>
+    <hyperlink ref="E8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="11" orientation="portrait" r:id="rId5"/>

</xml_diff>

<commit_message>
Ares 5 to 3.3*
</commit_message>
<xml_diff>
--- a/Presentation/feuille de course.xlsx
+++ b/Presentation/feuille de course.xlsx
@@ -168,13 +168,19 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -307,7 +313,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -333,6 +339,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -641,7 +652,7 @@
   <dimension ref="B2:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,7 +685,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
@@ -695,23 +706,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+    <row r="4" spans="2:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="21">
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="23">
         <v>0.76400000000000001</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="23">
         <f t="shared" ref="G4:G15" si="0">F4*C4</f>
         <v>0.76400000000000001</v>
       </c>
@@ -737,7 +748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>16</v>
       </c>
@@ -860,21 +871,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="8" t="s">
+    <row r="13" spans="2:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="21">
         <v>3</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14">
+      <c r="F13" s="23"/>
+      <c r="G13" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>

</xml_diff>